<commit_message>
Update Excel with UserStories
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Desktop\Switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruimiguelborges/Documents/ISEP/bitbucket-workspace/switch-2017-g003/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31AC2D1D-5263-4042-9E1D-5725C3F8247D}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4540" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="77">
   <si>
     <t>Sprint</t>
   </si>
@@ -250,6 +251,30 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>S7 (S2 2ªsem)</t>
+  </si>
+  <si>
+    <t>US103 - Como Administrador, quero que seja verificada a autenticidade dos novos utilizadores através do envio de um email ou SMS com um código de confirmação.</t>
+  </si>
+  <si>
+    <t>US105 - Como Administrador, quero que a aplicação carregue contas de utilizadores a partir de um ficheiro XML. Os utilizadores devem criar uma password a primeira vez que fizerem login. No primeiro login deve ser usado um mecanismo de autenticação alternativo: efetuar uma pergunta de segurança, enviar SMS com código para telefone, enviar email, etc.</t>
+  </si>
+  <si>
+    <t>US310 - Como Diretor, quero poder definir quais os mecanismos de cálculo de custo aplicáveis ao projeto.</t>
+  </si>
+  <si>
+    <t>US392 - Como Gestor de projeto, quero poder escolher o mecanismo de cálculo de custo, nomeadamente o que fazer quando os períodos de reporting não coincidem com os de custos dos colaboradores.</t>
+  </si>
+  <si>
+    <t>US901 v2 - Como Product Owner, quero que a aplicação carregue dados de teste a partir de um dos formatos de ficheiro XML disponibilizados.</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>US902 - Como Product Owner, quero que seja implementada uma API REST para as seguintes user stories: US136, US203, US204, US207, US370, US372, US390, US392</t>
   </si>
 </sst>
 </file>
@@ -315,7 +340,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +377,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -365,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="38">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -456,6 +487,27 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +533,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -777,25 +829,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D57" sqref="D57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="19"/>
-    <col min="2" max="2" width="14.42578125" style="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="164.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="19"/>
+    <col min="2" max="2" width="14.5" style="1"/>
+    <col min="3" max="3" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="164.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="1"/>
+    <col min="6" max="6" width="0.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -811,7 +863,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -827,7 +879,7 @@
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -843,7 +895,7 @@
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -859,7 +911,7 @@
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -875,7 +927,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
@@ -891,7 +943,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
@@ -907,7 +959,7 @@
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -923,7 +975,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
@@ -939,7 +991,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
@@ -955,7 +1007,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>1</v>
       </c>
@@ -971,7 +1023,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1039,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1055,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1071,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1087,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1103,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>12</v>
       </c>
@@ -1067,7 +1119,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1135,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1151,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>12</v>
       </c>
@@ -1115,7 +1167,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1183,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>12</v>
       </c>
@@ -1147,7 +1199,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
@@ -1163,7 +1215,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1231,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1247,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1263,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1279,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1295,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1311,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>22</v>
       </c>
@@ -1275,7 +1327,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1343,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>22</v>
       </c>
@@ -1307,7 +1359,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1375,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="16" t="s">
         <v>22</v>
       </c>
@@ -1339,7 +1391,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="16" t="s">
         <v>22</v>
       </c>
@@ -1355,7 +1407,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1423,7 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1439,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>34</v>
       </c>
@@ -1403,7 +1455,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>34</v>
       </c>
@@ -1419,7 +1471,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1487,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="17" t="s">
         <v>34</v>
       </c>
@@ -1451,7 +1503,7 @@
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>34</v>
       </c>
@@ -1467,7 +1519,7 @@
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
         <v>42</v>
       </c>
@@ -1483,7 +1535,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="18" t="s">
         <v>42</v>
       </c>
@@ -1499,7 +1551,7 @@
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
         <v>42</v>
       </c>
@@ -1515,7 +1567,7 @@
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
         <v>42</v>
       </c>
@@ -1531,7 +1583,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="18" t="s">
         <v>42</v>
       </c>
@@ -1547,7 +1599,7 @@
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
         <v>42</v>
       </c>
@@ -1563,7 +1615,7 @@
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
         <v>42</v>
       </c>
@@ -1579,7 +1631,7 @@
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
     </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="18" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1647,7 @@
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +1663,7 @@
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="18" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1679,7 @@
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="18" t="s">
         <v>42</v>
       </c>
@@ -1643,7 +1695,7 @@
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>42</v>
       </c>
@@ -1658,6 +1710,86 @@
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="36" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="37" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="35" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="36" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="36" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C59" s="34"/>
+      <c r="D59" s="36" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="35" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="34"/>
+      <c r="D60" s="36" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{011E32B1-0233-4759-92BB-9F6663E78B5D}"/>

</xml_diff>

<commit_message>
Update Excel with User Stories (master)
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18730"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10319"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Utilizador\Desktop\Switch\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruimiguelborges/Documents/ISEP/bitbucket-workspace/switch-2017-g003/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DAAAD4E-F7F9-0245-8A47-439EAD52BC0B}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="11520" windowHeight="7530" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4540" yWindow="-21600" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="77">
   <si>
     <t>Sprint</t>
   </si>
@@ -250,6 +251,30 @@
       </rPr>
       <t xml:space="preserve"> </t>
     </r>
+  </si>
+  <si>
+    <t>S7 (S2 2ªsem)</t>
+  </si>
+  <si>
+    <t>US103 - Como Administrador, quero que seja verificada a autenticidade dos novos utilizadores através do envio de um email ou SMS com um código de confirmação.</t>
+  </si>
+  <si>
+    <t>US105 - Como Administrador, quero que a aplicação carregue contas de utilizadores a partir de um ficheiro XML. Os utilizadores devem criar uma password a primeira vez que fizerem login. No primeiro login deve ser usado um mecanismo de autenticação alternativo: efetuar uma pergunta de segurança, enviar SMS com código para telefone, enviar email, etc.</t>
+  </si>
+  <si>
+    <t>US310 - Como Diretor, quero poder definir quais os mecanismos de cálculo de custo aplicáveis ao projeto.</t>
+  </si>
+  <si>
+    <t>US392 - Como Gestor de projeto, quero poder escolher o mecanismo de cálculo de custo, nomeadamente o que fazer quando os períodos de reporting não coincidem com os de custos dos colaboradores.</t>
+  </si>
+  <si>
+    <t>PO</t>
+  </si>
+  <si>
+    <t>US901 v2 - Como Product Owner, quero que a aplicação carregue dados de teste a partir de um dos formatos de ficheiro XML disponibilizados.</t>
+  </si>
+  <si>
+    <t>US902 - Como Product Owner, quero que seja implementada uma API REST para as seguintes user stories: US136, US203, US204, US207, US370, US372, US390, US392</t>
   </si>
 </sst>
 </file>
@@ -315,7 +340,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -352,6 +377,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -365,7 +396,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -456,6 +487,21 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -481,7 +527,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -777,25 +823,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F54"/>
+  <dimension ref="A1:F60"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="73" zoomScaleNormal="73" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A28" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C60" sqref="C60"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="14.42578125" style="19"/>
-    <col min="2" max="2" width="14.42578125" style="1"/>
-    <col min="3" max="3" width="21.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="164.140625" style="1" customWidth="1"/>
+    <col min="1" max="1" width="14.5" style="19"/>
+    <col min="2" max="2" width="14.5" style="1"/>
+    <col min="3" max="3" width="21.83203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="164.1640625" style="1" customWidth="1"/>
     <col min="5" max="5" width="13" style="1" customWidth="1"/>
-    <col min="6" max="6" width="0.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="16384" width="14.42578125" style="1"/>
+    <col min="6" max="6" width="0.5" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="16384" width="14.5" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:6" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
@@ -811,7 +857,7 @@
       <c r="E1" s="21"/>
       <c r="F1" s="21"/>
     </row>
-    <row r="2" spans="1:6" ht="27" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="28" x14ac:dyDescent="0.15">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -827,7 +873,7 @@
       <c r="E2" s="21"/>
       <c r="F2" s="21"/>
     </row>
-    <row r="3" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A3" s="14" t="s">
         <v>1</v>
       </c>
@@ -843,7 +889,7 @@
       <c r="E3" s="22"/>
       <c r="F3" s="22"/>
     </row>
-    <row r="4" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A4" s="14" t="s">
         <v>1</v>
       </c>
@@ -859,7 +905,7 @@
       <c r="E4" s="22"/>
       <c r="F4" s="22"/>
     </row>
-    <row r="5" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A5" s="14" t="s">
         <v>1</v>
       </c>
@@ -875,7 +921,7 @@
       <c r="E5" s="22"/>
       <c r="F5" s="22"/>
     </row>
-    <row r="6" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>1</v>
       </c>
@@ -891,7 +937,7 @@
       <c r="E6" s="22"/>
       <c r="F6" s="22"/>
     </row>
-    <row r="7" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A7" s="14" t="s">
         <v>1</v>
       </c>
@@ -907,7 +953,7 @@
       <c r="E7" s="22"/>
       <c r="F7" s="22"/>
     </row>
-    <row r="8" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A8" s="14" t="s">
         <v>1</v>
       </c>
@@ -923,7 +969,7 @@
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
     </row>
-    <row r="9" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A9" s="14" t="s">
         <v>1</v>
       </c>
@@ -939,7 +985,7 @@
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
     </row>
-    <row r="10" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A10" s="14" t="s">
         <v>1</v>
       </c>
@@ -955,7 +1001,7 @@
       <c r="E10" s="22"/>
       <c r="F10" s="22"/>
     </row>
-    <row r="11" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A11" s="14" t="s">
         <v>1</v>
       </c>
@@ -971,7 +1017,7 @@
       <c r="E11" s="22"/>
       <c r="F11" s="22"/>
     </row>
-    <row r="12" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A12" s="15" t="s">
         <v>12</v>
       </c>
@@ -987,7 +1033,7 @@
       <c r="E12" s="22"/>
       <c r="F12" s="22"/>
     </row>
-    <row r="13" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A13" s="15" t="s">
         <v>12</v>
       </c>
@@ -1003,7 +1049,7 @@
       <c r="E13" s="22"/>
       <c r="F13" s="22"/>
     </row>
-    <row r="14" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A14" s="15" t="s">
         <v>12</v>
       </c>
@@ -1019,7 +1065,7 @@
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
     </row>
-    <row r="15" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A15" s="15" t="s">
         <v>12</v>
       </c>
@@ -1035,7 +1081,7 @@
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
-    <row r="16" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A16" s="15" t="s">
         <v>12</v>
       </c>
@@ -1051,7 +1097,7 @@
       <c r="E16" s="22"/>
       <c r="F16" s="22"/>
     </row>
-    <row r="17" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A17" s="15" t="s">
         <v>12</v>
       </c>
@@ -1067,7 +1113,7 @@
       <c r="E17" s="22"/>
       <c r="F17" s="22"/>
     </row>
-    <row r="18" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A18" s="15" t="s">
         <v>12</v>
       </c>
@@ -1083,7 +1129,7 @@
       <c r="E18" s="22"/>
       <c r="F18" s="22"/>
     </row>
-    <row r="19" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A19" s="15" t="s">
         <v>12</v>
       </c>
@@ -1099,7 +1145,7 @@
       <c r="E19" s="22"/>
       <c r="F19" s="22"/>
     </row>
-    <row r="20" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A20" s="15" t="s">
         <v>12</v>
       </c>
@@ -1115,7 +1161,7 @@
       <c r="E20" s="22"/>
       <c r="F20" s="22"/>
     </row>
-    <row r="21" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A21" s="15" t="s">
         <v>12</v>
       </c>
@@ -1131,7 +1177,7 @@
       <c r="E21" s="22"/>
       <c r="F21" s="22"/>
     </row>
-    <row r="22" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A22" s="15" t="s">
         <v>12</v>
       </c>
@@ -1147,7 +1193,7 @@
       <c r="E22" s="22"/>
       <c r="F22" s="22"/>
     </row>
-    <row r="23" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A23" s="16" t="s">
         <v>22</v>
       </c>
@@ -1163,7 +1209,7 @@
       <c r="E23" s="22"/>
       <c r="F23" s="22"/>
     </row>
-    <row r="24" spans="1:6" ht="49.5" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" ht="42" x14ac:dyDescent="0.15">
       <c r="A24" s="16" t="s">
         <v>22</v>
       </c>
@@ -1179,7 +1225,7 @@
       <c r="E24" s="22"/>
       <c r="F24" s="22"/>
     </row>
-    <row r="25" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A25" s="16" t="s">
         <v>22</v>
       </c>
@@ -1195,7 +1241,7 @@
       <c r="E25" s="22"/>
       <c r="F25" s="22"/>
     </row>
-    <row r="26" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A26" s="16" t="s">
         <v>22</v>
       </c>
@@ -1211,7 +1257,7 @@
       <c r="E26" s="22"/>
       <c r="F26" s="22"/>
     </row>
-    <row r="27" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A27" s="16" t="s">
         <v>22</v>
       </c>
@@ -1227,7 +1273,7 @@
       <c r="E27" s="22"/>
       <c r="F27" s="22"/>
     </row>
-    <row r="28" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A28" s="16" t="s">
         <v>22</v>
       </c>
@@ -1243,7 +1289,7 @@
       <c r="E28" s="22"/>
       <c r="F28" s="22"/>
     </row>
-    <row r="29" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A29" s="16" t="s">
         <v>22</v>
       </c>
@@ -1259,7 +1305,7 @@
       <c r="E29" s="22"/>
       <c r="F29" s="22"/>
     </row>
-    <row r="30" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A30" s="16" t="s">
         <v>22</v>
       </c>
@@ -1275,7 +1321,7 @@
       <c r="E30" s="22"/>
       <c r="F30" s="22"/>
     </row>
-    <row r="31" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A31" s="16" t="s">
         <v>22</v>
       </c>
@@ -1291,7 +1337,7 @@
       <c r="E31" s="22"/>
       <c r="F31" s="22"/>
     </row>
-    <row r="32" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A32" s="16" t="s">
         <v>22</v>
       </c>
@@ -1307,7 +1353,7 @@
       <c r="E32" s="22"/>
       <c r="F32" s="22"/>
     </row>
-    <row r="33" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A33" s="16" t="s">
         <v>22</v>
       </c>
@@ -1323,7 +1369,7 @@
       <c r="E33" s="22"/>
       <c r="F33" s="22"/>
     </row>
-    <row r="34" spans="1:6" ht="33" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A34" s="16" t="s">
         <v>22</v>
       </c>
@@ -1339,7 +1385,7 @@
       <c r="E34" s="22"/>
       <c r="F34" s="22"/>
     </row>
-    <row r="35" spans="1:6" ht="16.5" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:6" ht="16" x14ac:dyDescent="0.15">
       <c r="A35" s="16" t="s">
         <v>22</v>
       </c>
@@ -1355,7 +1401,7 @@
       <c r="E35" s="22"/>
       <c r="F35" s="22"/>
     </row>
-    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A36" s="17" t="s">
         <v>34</v>
       </c>
@@ -1371,7 +1417,7 @@
       <c r="E36" s="22"/>
       <c r="F36" s="22"/>
     </row>
-    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A37" s="17" t="s">
         <v>34</v>
       </c>
@@ -1387,7 +1433,7 @@
       <c r="E37" s="22"/>
       <c r="F37" s="22"/>
     </row>
-    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A38" s="17" t="s">
         <v>34</v>
       </c>
@@ -1403,7 +1449,7 @@
       <c r="E38" s="22"/>
       <c r="F38" s="22"/>
     </row>
-    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="17" t="s">
         <v>34</v>
       </c>
@@ -1419,7 +1465,7 @@
       <c r="E39" s="22"/>
       <c r="F39" s="22"/>
     </row>
-    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>34</v>
       </c>
@@ -1435,7 +1481,7 @@
       <c r="E40" s="22"/>
       <c r="F40" s="22"/>
     </row>
-    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A41" s="17" t="s">
         <v>34</v>
       </c>
@@ -1451,7 +1497,7 @@
       <c r="E41" s="22"/>
       <c r="F41" s="22"/>
     </row>
-    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A42" s="17" t="s">
         <v>34</v>
       </c>
@@ -1467,7 +1513,7 @@
       <c r="E42" s="22"/>
       <c r="F42" s="22"/>
     </row>
-    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A43" s="18" t="s">
         <v>42</v>
       </c>
@@ -1483,7 +1529,7 @@
       <c r="E43" s="22"/>
       <c r="F43" s="22"/>
     </row>
-    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A44" s="18" t="s">
         <v>42</v>
       </c>
@@ -1499,7 +1545,7 @@
       <c r="E44" s="22"/>
       <c r="F44" s="22"/>
     </row>
-    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A45" s="18" t="s">
         <v>42</v>
       </c>
@@ -1515,7 +1561,7 @@
       <c r="E45" s="22"/>
       <c r="F45" s="22"/>
     </row>
-    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A46" s="18" t="s">
         <v>42</v>
       </c>
@@ -1531,7 +1577,7 @@
       <c r="E46" s="22"/>
       <c r="F46" s="22"/>
     </row>
-    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A47" s="18" t="s">
         <v>42</v>
       </c>
@@ -1547,7 +1593,7 @@
       <c r="E47" s="22"/>
       <c r="F47" s="22"/>
     </row>
-    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A48" s="18" t="s">
         <v>42</v>
       </c>
@@ -1563,7 +1609,7 @@
       <c r="E48" s="22"/>
       <c r="F48" s="22"/>
     </row>
-    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A49" s="18" t="s">
         <v>42</v>
       </c>
@@ -1579,7 +1625,7 @@
       <c r="E49" s="22"/>
       <c r="F49" s="22"/>
     </row>
-    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A50" s="18" t="s">
         <v>42</v>
       </c>
@@ -1595,7 +1641,7 @@
       <c r="E50" s="22"/>
       <c r="F50" s="22"/>
     </row>
-    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A51" s="18" t="s">
         <v>42</v>
       </c>
@@ -1611,7 +1657,7 @@
       <c r="E51" s="22"/>
       <c r="F51" s="22"/>
     </row>
-    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A52" s="18" t="s">
         <v>42</v>
       </c>
@@ -1627,7 +1673,7 @@
       <c r="E52" s="22"/>
       <c r="F52" s="22"/>
     </row>
-    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A53" s="18" t="s">
         <v>42</v>
       </c>
@@ -1643,7 +1689,7 @@
       <c r="E53" s="22"/>
       <c r="F53" s="22"/>
     </row>
-    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A54" s="18" t="s">
         <v>42</v>
       </c>
@@ -1658,6 +1704,86 @@
       </c>
       <c r="E54" s="22"/>
       <c r="F54" s="22"/>
+    </row>
+    <row r="55" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A55" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B55" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C55" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D55" s="34" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" ht="30" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A56" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="C56" s="33" t="s">
+        <v>65</v>
+      </c>
+      <c r="D56" s="35" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A57" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B57" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="C57" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D57" s="34" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A58" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B58" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="C58" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="D58" s="34" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A59" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B59" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="33"/>
+      <c r="D59" s="34" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A60" s="31" t="s">
+        <v>69</v>
+      </c>
+      <c r="B60" s="32" t="s">
+        <v>74</v>
+      </c>
+      <c r="C60" s="33"/>
+      <c r="D60" s="34" t="s">
+        <v>76</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A1:D1" xr:uid="{011E32B1-0233-4759-92BB-9F6663E78B5D}"/>

</xml_diff>

<commit_message>
addresses #153 update UserStories.xlsx file
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritamachado/switch-2017-g003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D1DD8916-5DA2-7F46-A5A3-E53476B6809A}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29508F50-2D36-8249-ABED-5F2DCB0C7B52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="ReactUI_completed" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$I$60</definedName>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="336" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="111">
   <si>
     <t>Sprint</t>
   </si>
@@ -315,12 +316,75 @@
   <si>
     <t>DELETE</t>
   </si>
+  <si>
+    <t>US101</t>
+  </si>
+  <si>
+    <t>US203</t>
+  </si>
+  <si>
+    <t>US205</t>
+  </si>
+  <si>
+    <t>US207</t>
+  </si>
+  <si>
+    <t>US390</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Como colaborador, eu pretendo consultar a minha lista de tarefas pendentes de modo a saber o que tenho para fazer hoje.</t>
+  </si>
+  <si>
+    <t>Como colaborador, eu pretendo marcar uma tarefa que consta na minha lista de tarefas como concluída.</t>
+  </si>
+  <si>
+    <t>Como colaborador, eu pretendo registar/atualizar o tempo despendido numa tarefa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Como Gestor de projeto quero poder calcular o custo total reportado no projeto até ao momento</t>
+  </si>
+  <si>
+    <t>US320</t>
+  </si>
+  <si>
+    <t>Lista de Projetos ativos</t>
+  </si>
+  <si>
+    <t>mostar users</t>
+  </si>
+  <si>
+    <t>US130</t>
+  </si>
+  <si>
+    <t>S2 Sprint4</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Registo de Utilizador</t>
+  </si>
+  <si>
+    <t>completed</t>
+  </si>
+  <si>
+    <t>Mandatory</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -384,8 +448,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF333333"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -428,11 +512,62 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -441,7 +576,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -564,6 +699,31 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -887,11 +1047,11 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr filterMode="1"/>
-  <dimension ref="A1:I60"/>
+  <dimension ref="A1:I76"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D45" sqref="D45"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2175,6 +2335,71 @@
         <v>76</v>
       </c>
     </row>
+    <row r="64" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B64" s="43"/>
+      <c r="C64" s="43"/>
+      <c r="D64" s="43"/>
+    </row>
+    <row r="65" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B65" s="43"/>
+      <c r="C65" s="43"/>
+      <c r="D65" s="43"/>
+    </row>
+    <row r="66" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B66" s="43"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="45"/>
+    </row>
+    <row r="67" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B67" s="43"/>
+      <c r="C67" s="44"/>
+      <c r="D67" s="43"/>
+    </row>
+    <row r="68" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B68" s="43"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="43"/>
+    </row>
+    <row r="69" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B69" s="43"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="45"/>
+    </row>
+    <row r="70" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="B70" s="43"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="43"/>
+    </row>
+    <row r="71" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B71" s="43"/>
+      <c r="C71" s="45"/>
+      <c r="D71" s="45"/>
+    </row>
+    <row r="72" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B72" s="43"/>
+      <c r="C72" s="45"/>
+      <c r="D72" s="45"/>
+    </row>
+    <row r="73" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B73" s="43"/>
+      <c r="C73" s="43"/>
+      <c r="D73" s="43"/>
+    </row>
+    <row r="74" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B74" s="43"/>
+      <c r="C74" s="43"/>
+      <c r="D74" s="43"/>
+    </row>
+    <row r="75" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B75" s="43"/>
+      <c r="C75" s="43"/>
+      <c r="D75" s="43"/>
+    </row>
+    <row r="76" spans="2:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="B76" s="43"/>
+      <c r="C76" s="43"/>
+      <c r="D76" s="43"/>
+    </row>
   </sheetData>
   <autoFilter ref="A1:I60" xr:uid="{EA6A7D03-B76A-9141-A024-F3683425519C}">
     <filterColumn colId="4">
@@ -2192,4 +2417,129 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9166912A-7BB2-964D-9D73-7F5BE8A06B40}">
+  <dimension ref="A2:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="1" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="119.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:4" ht="33" x14ac:dyDescent="0.15">
+      <c r="A2" s="42" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" s="42" t="s">
+        <v>104</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A3" s="46" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="47" t="s">
+        <v>106</v>
+      </c>
+      <c r="C3" s="47"/>
+      <c r="D3" s="47" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A4" s="46" t="s">
+        <v>91</v>
+      </c>
+      <c r="B4" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A5" s="46" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="48" t="s">
+        <v>96</v>
+      </c>
+      <c r="C5" s="48" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A6" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="B6" s="48" t="s">
+        <v>97</v>
+      </c>
+      <c r="C6" s="48"/>
+      <c r="D6" s="48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A7" s="46" t="s">
+        <v>94</v>
+      </c>
+      <c r="B7" s="48" t="s">
+        <v>98</v>
+      </c>
+      <c r="C7" s="48"/>
+      <c r="D7" s="48" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A8" s="49" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="50" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D8" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.15">
+      <c r="A9" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="B9" s="50" t="s">
+        <v>101</v>
+      </c>
+      <c r="C9" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D9" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
addresses #170 update UserStories.xlsx file
</commit_message>
<xml_diff>
--- a/UserStories.xlsx
+++ b/UserStories.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10410"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ritamachado/switch-2017-g003/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/ruimiguelborges/Documents/ISEP/bitbucket-workspace/switch-2017-g003/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29508F50-2D36-8249-ABED-5F2DCB0C7B52}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26D37FFA-21EC-C74E-918B-A143E5101769}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16740" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="369" uniqueCount="113">
   <si>
     <t>Sprint</t>
   </si>
@@ -378,6 +378,12 @@
   </si>
   <si>
     <t>no</t>
+  </si>
+  <si>
+    <t>Como Gestor de projeto, quero poder escolher o mecanismo de cálculo de custo, nomeadamente o que fazer quando os períodos de reporting não coincidem com os de custos dos colaboradores.</t>
+  </si>
+  <si>
+    <t>US 392</t>
   </si>
 </sst>
 </file>
@@ -576,7 +582,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="51">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -725,6 +731,9 @@
     </xf>
     <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1051,7 +1060,7 @@
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A47" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D76" sqref="D76"/>
+      <selection pane="bottomLeft" activeCell="D66" sqref="D66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2421,10 +2430,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9166912A-7BB2-964D-9D73-7F5BE8A06B40}">
-  <dimension ref="A2:D9"/>
+  <dimension ref="A2:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -2506,7 +2515,9 @@
       <c r="B7" s="48" t="s">
         <v>98</v>
       </c>
-      <c r="C7" s="48"/>
+      <c r="C7" s="48" t="s">
+        <v>107</v>
+      </c>
       <c r="D7" s="48" t="s">
         <v>109</v>
       </c>
@@ -2536,6 +2547,20 @@
         <v>107</v>
       </c>
       <c r="D9" s="50" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="38" x14ac:dyDescent="0.15">
+      <c r="A10" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="B10" s="51" t="s">
+        <v>111</v>
+      </c>
+      <c r="C10" s="50" t="s">
+        <v>107</v>
+      </c>
+      <c r="D10" s="50" t="s">
         <v>110</v>
       </c>
     </row>

</xml_diff>